<commit_message>
Minimal model run example
</commit_message>
<xml_diff>
--- a/Data/CTL_parameters.xlsx
+++ b/Data/CTL_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michelle.Sculley\Documents\OpenScienceTraining\ISC_OSworkflow_training_dev\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7651665-8DD6-4336-8425-BE3B21AB29C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A8CDCC-9C99-4B21-8B8A-3B08D764360D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32220" yWindow="705" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="16440" windowHeight="8655" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SWO" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="180">
   <si>
     <t>X1</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>Growth</t>
+  </si>
+  <si>
+    <t>SEL</t>
   </si>
 </sst>
 </file>
@@ -603,7 +606,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +667,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -677,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -703,6 +718,8 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4769,8 +4786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB86EC-F98E-46C7-A441-180557FBE943}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="78" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6301,7 +6318,7 @@
       <c r="A30" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -6354,7 +6371,7 @@
       <c r="A31" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -6407,7 +6424,7 @@
       <c r="A32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -6460,8 +6477,8 @@
       <c r="A33" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>19</v>
+      <c r="B33" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>20</v>
@@ -6513,8 +6530,8 @@
       <c r="A34" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>19</v>
+      <c r="B34" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>20</v>
@@ -6566,8 +6583,8 @@
       <c r="A35" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>19</v>
+      <c r="B35" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>20</v>
@@ -6619,8 +6636,8 @@
       <c r="A36" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>19</v>
+      <c r="B36" s="19" t="s">
+        <v>179</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>

</xml_diff>